<commit_message>
se configuro motor widget
</commit_message>
<xml_diff>
--- a/datos del negocio.xlsx
+++ b/datos del negocio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>